<commit_message>
Update Excel file from Jenkins job
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹11,444 per gram for 24 karat gold, ₹10,490 per gram for 22 karat gold and ₹8,583 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>26-09-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹11,488 per gram for 24 karat gold, ₹10,530 per gram for 22 karat gold and ₹8,616 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -449,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -494,6 +500,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from Jenkins job 1
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -455,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -508,6 +508,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -455,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -516,6 +516,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s" s="4">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-09-26 11:44:32
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -455,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -572,6 +572,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s" s="4">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-09-27 06:24:33
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Javaproject\GoldPriceandStockNews\src\test\resources\Data\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -54,12 +54,19 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹11,488 per gram for 24 karat gold, ₹10,530 per gram for 22 karat gold and ₹8,616 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>27-09-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹11,548 per gram for 24 karat gold, ₹10,585 per gram for 22 karat gold and ₹8,661 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -454,7 +461,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -462,9 +469,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="94.6640625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" customWidth="true" style="3" width="13.109375"/>
+    <col min="2" max="2" customWidth="true" style="4" width="94.6640625"/>
+    <col min="3" max="16384" style="3" width="8.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -507,6 +514,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-09-28 06:26:30
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹11,548 per gram for 24 karat gold, ₹10,585 per gram for 22 karat gold and ₹8,661 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>28-09-2025</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -522,6 +525,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s" s="4">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-09-29 06:31:22
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>28-09-2025</t>
+  </si>
+  <si>
+    <t>29-09-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹11,640 per gram for 24 karat gold, ₹10,670 per gram for 22 karat gold and ₹8,730 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -464,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -533,6 +539,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s" s="4">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-09-30 06:29:11
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹11,640 per gram for 24 karat gold, ₹10,670 per gram for 22 karat gold and ₹8,730 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>30-09-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹11,831 per gram for 24 karat gold, ₹10,845 per gram for 22 karat gold and ₹8,873 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -470,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -547,6 +553,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-01 06:28:56
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹11,831 per gram for 24 karat gold, ₹10,845 per gram for 22 karat gold and ₹8,873 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>01-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹11,864 per gram for 24 karat gold, ₹10,875 per gram for 22 karat gold and ₹8,898 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -476,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -561,6 +567,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s" s="4">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-02 06:29:31
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹11,864 per gram for 24 karat gold, ₹10,875 per gram for 22 karat gold and ₹8,898 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>02-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹11,869 per gram for 24 karat gold, ₹10,880 per gram for 22 karat gold and ₹8,902 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -575,6 +581,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s" s="4">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-03 06:27:43
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹11,869 per gram for 24 karat gold, ₹10,880 per gram for 22 karat gold and ₹8,902 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>03-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹11,804 per gram for 24 karat gold, ₹10,820 per gram for 22 karat gold and ₹8,853 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -589,6 +595,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s" s="4">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-04 06:27:00
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹11,804 per gram for 24 karat gold, ₹10,820 per gram for 22 karat gold and ₹8,853 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>04-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹11,940 per gram for 24 karat gold, ₹10,945 per gram for 22 karat gold and ₹8,955 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -603,6 +609,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s" s="4">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-05 06:25:39
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹11,940 per gram for 24 karat gold, ₹10,945 per gram for 22 karat gold and ₹8,955 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>05-10-2025</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -617,6 +620,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s" s="4">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-06 06:29:27
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>05-10-2025</t>
+  </si>
+  <si>
+    <t>06-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,077 per gram for 24 karat gold, ₹11,070 per gram for 22 karat gold and ₹9,058 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -503,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -628,6 +634,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s" s="4">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-07 06:28:32
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,077 per gram for 24 karat gold, ₹11,070 per gram for 22 karat gold and ₹9,058 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>07-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,202 per gram for 24 karat gold, ₹11,185 per gram for 22 karat gold and ₹9,152 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -509,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -642,6 +648,14 @@
         <v>23</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s" s="4">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-08 06:29:13
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,202 per gram for 24 karat gold, ₹11,185 per gram for 22 karat gold and ₹9,152 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>08-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,317 per gram for 24 karat gold, ₹11,290 per gram for 22 karat gold and ₹9,238 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -515,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -656,6 +662,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s" s="4">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-09 06:29:46
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,317 per gram for 24 karat gold, ₹11,290 per gram for 22 karat gold and ₹9,238 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>09-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,415 per gram for 24 karat gold, ₹11,380 per gram for 22 karat gold and ₹9,311 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -521,7 +527,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -670,6 +676,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s" s="4">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-10 06:29:29
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,415 per gram for 24 karat gold, ₹11,380 per gram for 22 karat gold and ₹9,311 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>10-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,229 per gram for 24 karat gold, ₹11,210 per gram for 22 karat gold and ₹9,172 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -527,7 +533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -684,6 +690,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s" s="4">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-11 06:25:45
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,229 per gram for 24 karat gold, ₹11,210 per gram for 22 karat gold and ₹9,172 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>11-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,426 per gram for 24 karat gold, ₹11,390 per gram for 22 karat gold and ₹9,319 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -533,7 +539,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -698,6 +704,14 @@
         <v>31</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s" s="4">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-12 06:25:44
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,426 per gram for 24 karat gold, ₹11,390 per gram for 22 karat gold and ₹9,319 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>12-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,508 per gram for 24 karat gold, ₹11,465 per gram for 22 karat gold and ₹9,381 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -539,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -712,6 +718,14 @@
         <v>33</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="s" s="3">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s" s="4">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-13 06:31:58
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,508 per gram for 24 karat gold, ₹11,465 per gram for 22 karat gold and ₹9,381 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>13-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,540 per gram for 24 karat gold, ₹11,495 per gram for 22 karat gold and ₹9,405 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -726,6 +732,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="s" s="3">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s" s="4">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-14 06:29:12
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,540 per gram for 24 karat gold, ₹11,495 per gram for 22 karat gold and ₹9,405 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>14-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,868 per gram for 24 karat gold, ₹11,795 per gram for 22 karat gold and ₹9,651 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -551,7 +557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -740,6 +746,14 @@
         <v>37</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s" s="4">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-15 06:30:51
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,868 per gram for 24 karat gold, ₹11,795 per gram for 22 karat gold and ₹9,651 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>15-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,889 per gram for 24 karat gold, ₹11,815 per gram for 22 karat gold and ₹9,697 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -557,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -754,6 +760,14 @@
         <v>39</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="s" s="3">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s" s="4">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-16 06:29:06
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,889 per gram for 24 karat gold, ₹11,815 per gram for 22 karat gold and ₹9,697 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>16-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,944 per gram for 24 karat gold, ₹11,865 per gram for 22 karat gold and ₹9,708 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -563,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -768,6 +774,14 @@
         <v>41</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s" s="4">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-17 06:28:58
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,944 per gram for 24 karat gold, ₹11,865 per gram for 22 karat gold and ₹9,708 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>17-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,277 per gram for 24 karat gold, ₹12,170 per gram for 22 karat gold and ₹9,958 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -569,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -782,6 +788,14 @@
         <v>43</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="s" s="3">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s" s="4">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-18 06:26:16
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,277 per gram for 24 karat gold, ₹12,170 per gram for 22 karat gold and ₹9,958 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>18-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,086 per gram for 24 karat gold, ₹11,995 per gram for 22 karat gold and ₹9,814 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -796,6 +802,14 @@
         <v>45</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="s" s="3">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s" s="4">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-19 06:38:29
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,086 per gram for 24 karat gold, ₹11,995 per gram for 22 karat gold and ₹9,814 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>19-10-2025</t>
   </si>
 </sst>
 </file>
@@ -581,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -810,6 +813,14 @@
         <v>47</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="s" s="3">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s" s="4">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-20 06:30:54
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>19-10-2025</t>
+  </si>
+  <si>
+    <t>20-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,069 per gram for 24 karat gold, ₹11,980 per gram for 22 karat gold and ₹9,802 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -584,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -821,6 +827,14 @@
         <v>47</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="s" s="3">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s" s="4">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-21 06:29:11
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,069 per gram for 24 karat gold, ₹11,980 per gram for 22 karat gold and ₹9,802 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>21-10-2025</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -835,6 +838,14 @@
         <v>50</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="s" s="3">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s" s="4">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-22 06:30:35
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>21-10-2025</t>
+  </si>
+  <si>
+    <t>22-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,720 per gram for 24 karat gold, ₹11,660 per gram for 22 karat gold and ₹9,540 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -593,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -846,6 +852,14 @@
         <v>45</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="s" s="3">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s" s="4">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-23 06:29:32
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,720 per gram for 24 karat gold, ₹11,660 per gram for 22 karat gold and ₹9,540 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>23-10-2025</t>
   </si>
 </sst>
 </file>
@@ -599,7 +602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -860,6 +863,14 @@
         <v>53</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s" s="4">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-24 08:58:05
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -608,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -909,6 +909,14 @@
         <v>56</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="B37" t="s" s="4">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-24 10:16:26
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -608,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -917,6 +917,14 @@
         <v>56</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="B38" t="s" s="4">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-24 11:00:12
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -608,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -925,6 +925,14 @@
         <v>56</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s" s="4">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-24 11:17:57
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -608,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -933,6 +933,14 @@
         <v>56</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s" s="4">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-25 15:17:01
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,546 per gram for 24 karat gold, ₹11,500 per gram for 22 karat gold and ₹9,409 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>25-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,562 per gram for 24 karat gold, ₹11,515 per gram for 22 karat gold and ₹9,422 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -608,7 +614,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -941,6 +947,14 @@
         <v>56</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s" s="4">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-26 06:28:39
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,562 per gram for 24 karat gold, ₹11,515 per gram for 22 karat gold and ₹9,422 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>26-10-2025</t>
   </si>
 </sst>
 </file>
@@ -614,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -955,6 +958,14 @@
         <v>58</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s" s="4">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-27 06:34:19
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>26-10-2025</t>
+  </si>
+  <si>
+    <t>27-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,448 per gram for 24 karat gold, ₹11,410 per gram for 22 karat gold and ₹9,336 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -617,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -966,6 +972,14 @@
         <v>58</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="B43" t="s" s="4">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-28 06:32:27
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,448 per gram for 24 karat gold, ₹11,410 per gram for 22 karat gold and ₹9,336 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>28-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,246 per gram for 24 karat gold, ₹11,225 per gram for 22 karat gold and ₹9,184 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -623,7 +629,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -980,6 +986,14 @@
         <v>61</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="s" s="3">
+        <v>62</v>
+      </c>
+      <c r="B44" t="s" s="4">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-29 06:32:49
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,246 per gram for 24 karat gold, ₹11,225 per gram for 22 karat gold and ₹9,184 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>29-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,158 per gram for 24 karat gold, ₹11,145 per gram for 22 karat gold and ₹9,119 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -629,7 +635,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -994,6 +1000,14 @@
         <v>63</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="s" s="3">
+        <v>64</v>
+      </c>
+      <c r="B45" t="s" s="4">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-30 06:30:50
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,158 per gram for 24 karat gold, ₹11,145 per gram for 22 karat gold and ₹9,119 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>30-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,049 per gram for 24 karat gold, ₹11,045 per gram for 22 karat gold and ₹9,037 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -635,7 +641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1008,6 +1014,14 @@
         <v>65</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="s" s="3">
+        <v>66</v>
+      </c>
+      <c r="B46" t="s" s="4">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-10-31 06:31:33
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,049 per gram for 24 karat gold, ₹11,045 per gram for 22 karat gold and ₹9,037 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>31-10-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,268 per gram for 24 karat gold, ₹11,245 per gram for 22 karat gold and ₹9,201 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -641,7 +647,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1022,6 +1028,14 @@
         <v>67</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="B47" t="s" s="4">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-01 06:28:13
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,268 per gram for 24 karat gold, ₹11,245 per gram for 22 karat gold and ₹9,201 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>01-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,300 per gram for 24 karat gold, ₹11,275 per gram for 22 karat gold and ₹9,225 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -647,7 +653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1036,6 +1042,14 @@
         <v>69</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="s" s="3">
+        <v>70</v>
+      </c>
+      <c r="B48" t="s" s="4">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-02 06:29:26
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,300 per gram for 24 karat gold, ₹11,275 per gram for 22 karat gold and ₹9,225 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>02-11-2025</t>
   </si>
 </sst>
 </file>
@@ -653,7 +656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1050,6 +1053,14 @@
         <v>71</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="s" s="3">
+        <v>72</v>
+      </c>
+      <c r="B49" t="s" s="4">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-03 06:32:59
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>02-11-2025</t>
+  </si>
+  <si>
+    <t>03-11-2025</t>
   </si>
 </sst>
 </file>
@@ -656,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1061,6 +1064,14 @@
         <v>71</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="s" s="3">
+        <v>73</v>
+      </c>
+      <c r="B50" t="s" s="4">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-04 06:32:59
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>03-11-2025</t>
+  </si>
+  <si>
+    <t>04-11-2025</t>
   </si>
 </sst>
 </file>
@@ -659,7 +662,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1072,6 +1075,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="s" s="3">
+        <v>74</v>
+      </c>
+      <c r="B51" t="s" s="4">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-05 06:31:40
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>04-11-2025</t>
+  </si>
+  <si>
+    <t>05-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,148 per gram for 24 karat gold, ₹11,135 per gram for 22 karat gold and ₹9,111 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -662,7 +668,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1083,6 +1089,14 @@
         <v>63</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="s" s="3">
+        <v>75</v>
+      </c>
+      <c r="B52" t="s" s="4">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-06 06:31:33
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,148 per gram for 24 karat gold, ₹11,135 per gram for 22 karat gold and ₹9,111 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>06-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,191 per gram for 24 karat gold, ₹11,175 per gram for 22 karat gold and ₹9,143 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -668,7 +674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1097,6 +1103,14 @@
         <v>76</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="s" s="3">
+        <v>77</v>
+      </c>
+      <c r="B53" t="s" s="4">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-07 06:31:27
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,191 per gram for 24 karat gold, ₹11,175 per gram for 22 karat gold and ₹9,143 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>07-11-2025</t>
   </si>
 </sst>
 </file>
@@ -674,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1111,6 +1114,14 @@
         <v>78</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="s" s="3">
+        <v>79</v>
+      </c>
+      <c r="B54" t="s" s="4">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-10 11:27:27
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>07-11-2025</t>
+  </si>
+  <si>
+    <t>10-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,322 per gram for 24 karat gold, ₹11,295 per gram for 22 karat gold and ₹9,242 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -677,7 +683,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1122,6 +1128,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="s" s="3">
+        <v>80</v>
+      </c>
+      <c r="B55" t="s" s="4">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-11 06:32:03
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
   <si>
     <t>Date</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,322 per gram for 24 karat gold, ₹11,295 per gram for 22 karat gold and ₹9,242 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>11-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,628 per gram for 24 karat gold, ₹11,575 per gram for 22 karat gold and ₹9,471 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -683,7 +689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1136,6 +1142,14 @@
         <v>81</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="B56" t="s" s="4">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-12 06:32:20
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,628 per gram for 24 karat gold, ₹11,575 per gram for 22 karat gold and ₹9,471 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>12-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,551 per gram for 24 karat gold, ₹11,505 per gram for 22 karat gold and ₹9,413 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -689,7 +695,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1150,6 +1156,14 @@
         <v>83</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="s" s="3">
+        <v>84</v>
+      </c>
+      <c r="B57" t="s" s="4">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-13 06:32:35
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,551 per gram for 24 karat gold, ₹11,505 per gram for 22 karat gold and ₹9,413 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>13-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,780 per gram for 24 karat gold, ₹11,715 per gram for 22 karat gold and ₹9,585 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -695,7 +701,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1164,6 +1170,14 @@
         <v>85</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="s" s="3">
+        <v>86</v>
+      </c>
+      <c r="B58" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-14 06:32:31
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,780 per gram for 24 karat gold, ₹11,715 per gram for 22 karat gold and ₹9,585 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>14-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,785 per gram for 24 karat gold, ₹11,720 per gram for 22 karat gold and ₹9,589 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -701,7 +707,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1178,6 +1184,14 @@
         <v>87</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="B59" t="s" s="4">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-15 06:29:02
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,785 per gram for 24 karat gold, ₹11,720 per gram for 22 karat gold and ₹9,589 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>15-11-2025</t>
   </si>
 </sst>
 </file>
@@ -707,7 +710,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1192,6 +1195,14 @@
         <v>89</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="s" s="3">
+        <v>90</v>
+      </c>
+      <c r="B60" t="s" s="4">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-16 06:30:01
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>15-11-2025</t>
+  </si>
+  <si>
+    <t>16-11-2025</t>
   </si>
 </sst>
 </file>
@@ -710,7 +713,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1203,6 +1206,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="s" s="3">
+        <v>91</v>
+      </c>
+      <c r="B61" t="s" s="4">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-17 06:33:06
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>16-11-2025</t>
+  </si>
+  <si>
+    <t>17-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,497 per gram for 24 karat gold, ₹11,455 per gram for 22 karat gold and ₹9,373 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -713,7 +719,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1214,6 +1220,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="s" s="3">
+        <v>92</v>
+      </c>
+      <c r="B62" t="s" s="4">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-18 06:31:37
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,497 per gram for 24 karat gold, ₹11,455 per gram for 22 karat gold and ₹9,373 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>18-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,366 per gram for 24 karat gold, ₹11,335 per gram for 22 karat gold and ₹9,274 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -719,7 +725,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1228,6 +1234,14 @@
         <v>93</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="s" s="3">
+        <v>94</v>
+      </c>
+      <c r="B63" t="s" s="4">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-19 06:31:53
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
   <si>
     <t>Date</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,366 per gram for 24 karat gold, ₹11,335 per gram for 22 karat gold and ₹9,274 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>19-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,486 per gram for 24 karat gold, ₹11,445 per gram for 22 karat gold and ₹9,364 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -725,7 +731,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1242,6 +1248,14 @@
         <v>95</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="s" s="3">
+        <v>96</v>
+      </c>
+      <c r="B64" t="s" s="4">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-20 06:31:11
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,486 per gram for 24 karat gold, ₹11,445 per gram for 22 karat gold and ₹9,364 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>20-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,469 per gram for 24 karat gold, ₹11,430 per gram for 22 karat gold and ₹9,352 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -731,7 +737,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1256,6 +1262,14 @@
         <v>97</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="s" s="3">
+        <v>98</v>
+      </c>
+      <c r="B65" t="s" s="4">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-21 06:33:22
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
   <si>
     <t>Date</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,469 per gram for 24 karat gold, ₹11,430 per gram for 22 karat gold and ₹9,352 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>21-11-2025</t>
   </si>
 </sst>
 </file>
@@ -737,7 +740,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1270,6 +1273,14 @@
         <v>99</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="s" s="3">
+        <v>100</v>
+      </c>
+      <c r="B66" t="s" s="4">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-22 06:28:49
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="103">
   <si>
     <t>Date</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>21-11-2025</t>
+  </si>
+  <si>
+    <t>22-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,584 per gram for 24 karat gold, ₹11,535 per gram for 22 karat gold and ₹9,438 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -740,7 +746,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1281,6 +1287,14 @@
         <v>61</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="s" s="3">
+        <v>101</v>
+      </c>
+      <c r="B67" t="s" s="4">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-23 06:30:14
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
   <si>
     <t>Date</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,584 per gram for 24 karat gold, ₹11,535 per gram for 22 karat gold and ₹9,438 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>23-11-2025</t>
   </si>
 </sst>
 </file>
@@ -746,7 +749,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1295,6 +1298,14 @@
         <v>102</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="s" s="3">
+        <v>103</v>
+      </c>
+      <c r="B68" t="s" s="4">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-24 06:33:14
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>23-11-2025</t>
+  </si>
+  <si>
+    <t>24-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,513 per gram for 24 karat gold, ₹11,470 per gram for 22 karat gold and ₹9,385 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -749,7 +755,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1306,6 +1312,14 @@
         <v>102</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="s" s="3">
+        <v>104</v>
+      </c>
+      <c r="B69" t="s" s="4">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-25 06:33:47
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,513 per gram for 24 karat gold, ₹11,470 per gram for 22 karat gold and ₹9,385 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>25-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,704 per gram for 24 karat gold, ₹11,645 per gram for 22 karat gold and ₹9,528 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -755,7 +761,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1320,6 +1326,14 @@
         <v>105</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="s" s="3">
+        <v>106</v>
+      </c>
+      <c r="B70" t="s" s="4">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-26 06:33:15
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,704 per gram for 24 karat gold, ₹11,645 per gram for 22 karat gold and ₹9,528 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>26-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,791 per gram for 24 karat gold, ₹11,725 per gram for 22 karat gold and ₹9,593 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -761,7 +767,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1334,6 +1340,14 @@
         <v>107</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="s" s="3">
+        <v>108</v>
+      </c>
+      <c r="B71" t="s" s="4">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-27 06:34:41
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="112">
   <si>
     <t>Date</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,791 per gram for 24 karat gold, ₹11,725 per gram for 22 karat gold and ₹9,593 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>27-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,775 per gram for 24 karat gold, ₹11,710 per gram for 22 karat gold and ₹9,581 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -767,7 +773,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1348,6 +1354,14 @@
         <v>109</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="s" s="3">
+        <v>110</v>
+      </c>
+      <c r="B72" t="s" s="4">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-28 06:33:15
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="114">
   <si>
     <t>Date</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,775 per gram for 24 karat gold, ₹11,710 per gram for 22 karat gold and ₹9,581 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>28-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,846 per gram for 24 karat gold, ₹11,775 per gram for 22 karat gold and ₹9,634 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -773,7 +779,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1362,6 +1368,14 @@
         <v>111</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="s" s="3">
+        <v>112</v>
+      </c>
+      <c r="B73" t="s" s="4">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-29 06:30:21
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="116">
   <si>
     <t>Date</t>
   </si>
@@ -378,6 +378,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,846 per gram for 24 karat gold, ₹11,775 per gram for 22 karat gold and ₹9,634 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>29-11-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,982 per gram for 24 karat gold, ₹11,900 per gram for 22 karat gold and ₹9,737 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -779,7 +785,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1376,6 +1382,14 @@
         <v>113</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="s" s="3">
+        <v>114</v>
+      </c>
+      <c r="B74" t="s" s="4">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-11-30 06:31:48
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,982 per gram for 24 karat gold, ₹11,900 per gram for 22 karat gold and ₹9,737 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>30-11-2025</t>
   </si>
 </sst>
 </file>
@@ -785,7 +788,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1390,6 +1393,14 @@
         <v>115</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="s" s="3">
+        <v>116</v>
+      </c>
+      <c r="B75" t="s" s="4">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-01 06:35:35
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="119">
   <si>
     <t>Date</t>
   </si>
@@ -387,6 +387,12 @@
   </si>
   <si>
     <t>30-11-2025</t>
+  </si>
+  <si>
+    <t>01-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,048 per gram for 24 karat gold, ₹11,960 per gram for 22 karat gold and ₹9,786 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -788,7 +794,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1401,6 +1407,14 @@
         <v>115</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="s" s="3">
+        <v>117</v>
+      </c>
+      <c r="B76" t="s" s="4">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-02 06:35:11
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
   <si>
     <t>Date</t>
   </si>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,048 per gram for 24 karat gold, ₹11,960 per gram for 22 karat gold and ₹9,786 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>02-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,020 per gram for 24 karat gold, ₹11,935 per gram for 22 karat gold and ₹9,765 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -794,7 +800,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1415,6 +1421,14 @@
         <v>118</v>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" t="s" s="3">
+        <v>119</v>
+      </c>
+      <c r="B77" t="s" s="4">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-03 06:33:59
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
   <si>
     <t>Date</t>
   </si>
@@ -399,6 +399,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,020 per gram for 24 karat gold, ₹11,935 per gram for 22 karat gold and ₹9,765 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>03-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,058 per gram for 24 karat gold, ₹11,970 per gram for 22 karat gold and ₹9,794 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -800,7 +806,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1429,6 +1435,14 @@
         <v>120</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="s" s="3">
+        <v>121</v>
+      </c>
+      <c r="B78" t="s" s="4">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-04 06:34:20
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="125">
   <si>
     <t>Date</t>
   </si>
@@ -405,6 +405,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,058 per gram for 24 karat gold, ₹11,970 per gram for 22 karat gold and ₹9,794 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>04-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,036 per gram for 24 karat gold, ₹11,950 per gram for 22 karat gold and ₹9,778 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -806,7 +812,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1443,6 +1449,14 @@
         <v>122</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="s" s="3">
+        <v>123</v>
+      </c>
+      <c r="B79" t="s" s="4">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-05 06:34:08
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="127">
   <si>
     <t>Date</t>
   </si>
@@ -411,6 +411,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,036 per gram for 24 karat gold, ₹11,950 per gram for 22 karat gold and ₹9,778 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>05-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹12,993 per gram for 24 karat gold, ₹11,910 per gram for 22 karat gold and ₹9,745 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -812,7 +818,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1457,6 +1463,14 @@
         <v>124</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="s" s="3">
+        <v>125</v>
+      </c>
+      <c r="B80" t="s" s="4">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-06 06:30:12
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="129">
   <si>
     <t>Date</t>
   </si>
@@ -417,6 +417,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹12,993 per gram for 24 karat gold, ₹11,910 per gram for 22 karat gold and ₹9,745 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>06-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,015 per gram for 24 karat gold, ₹11,930 per gram for 22 karat gold and ₹9,761 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -818,7 +824,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1471,6 +1477,14 @@
         <v>126</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="s" s="3">
+        <v>127</v>
+      </c>
+      <c r="B81" t="s" s="4">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-07 06:29:58
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="130">
   <si>
     <t>Date</t>
   </si>
@@ -423,6 +423,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,015 per gram for 24 karat gold, ₹11,930 per gram for 22 karat gold and ₹9,761 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>07-12-2025</t>
   </si>
 </sst>
 </file>
@@ -824,7 +827,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1485,6 +1488,14 @@
         <v>128</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="s" s="3">
+        <v>129</v>
+      </c>
+      <c r="B82" t="s" s="4">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-08 06:36:42
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="132">
   <si>
     <t>Date</t>
   </si>
@@ -426,6 +426,12 @@
   </si>
   <si>
     <t>07-12-2025</t>
+  </si>
+  <si>
+    <t>08-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,042 per gram for 24 karat gold, ₹11,955 per gram for 22 karat gold and ₹9,782 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -827,7 +833,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1496,6 +1502,14 @@
         <v>128</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="s" s="3">
+        <v>130</v>
+      </c>
+      <c r="B83" t="s" s="4">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-09 06:34:41
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="134">
   <si>
     <t>Date</t>
   </si>
@@ -432,6 +432,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,042 per gram for 24 karat gold, ₹11,955 per gram for 22 karat gold and ₹9,782 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>09-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,009 per gram for 24 karat gold, ₹11,925 per gram for 22 karat gold and ₹9,757 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -833,7 +839,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1510,6 +1516,14 @@
         <v>131</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="s" s="3">
+        <v>132</v>
+      </c>
+      <c r="B84" t="s" s="4">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-10 06:35:19
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="136">
   <si>
     <t>Date</t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,009 per gram for 24 karat gold, ₹11,925 per gram for 22 karat gold and ₹9,757 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>10-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,031 per gram for 24 karat gold, ₹11,945 per gram for 22 karat gold and ₹9,773 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -839,7 +845,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1524,6 +1530,14 @@
         <v>133</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="s" s="3">
+        <v>134</v>
+      </c>
+      <c r="B85" t="s" s="4">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-11 06:36:33
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="137">
   <si>
     <t>Date</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,031 per gram for 24 karat gold, ₹11,945 per gram for 22 karat gold and ₹9,773 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>11-12-2025</t>
   </si>
 </sst>
 </file>
@@ -845,7 +848,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B85"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1538,6 +1541,14 @@
         <v>135</v>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="s" s="3">
+        <v>136</v>
+      </c>
+      <c r="B86" t="s" s="4">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-12 06:35:01
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="139">
   <si>
     <t>Date</t>
   </si>
@@ -447,6 +447,12 @@
   </si>
   <si>
     <t>11-12-2025</t>
+  </si>
+  <si>
+    <t>12-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,266 per gram for 24 karat gold, ₹12,160 per gram for 22 karat gold and ₹9,949 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -848,7 +854,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1549,6 +1555,14 @@
         <v>120</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="s" s="3">
+        <v>137</v>
+      </c>
+      <c r="B87" t="s" s="4">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-13 06:32:30
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="141">
   <si>
     <t>Date</t>
   </si>
@@ -453,6 +453,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,266 per gram for 24 karat gold, ₹12,160 per gram for 22 karat gold and ₹9,949 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>13-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,391 per gram for 24 karat gold, ₹12,275 per gram for 22 karat gold and ₹10,043 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -854,7 +860,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B87"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1563,6 +1569,14 @@
         <v>138</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="s" s="3">
+        <v>139</v>
+      </c>
+      <c r="B88" t="s" s="4">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-14 06:31:54
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="142">
   <si>
     <t>Date</t>
   </si>
@@ -459,6 +459,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,391 per gram for 24 karat gold, ₹12,275 per gram for 22 karat gold and ₹10,043 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>14-12-2025</t>
   </si>
 </sst>
 </file>
@@ -860,7 +863,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1577,6 +1580,14 @@
         <v>140</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="s" s="3">
+        <v>141</v>
+      </c>
+      <c r="B89" t="s" s="4">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-15 06:38:08
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="144">
   <si>
     <t>Date</t>
   </si>
@@ -462,6 +462,12 @@
   </si>
   <si>
     <t>14-12-2025</t>
+  </si>
+  <si>
+    <t>15-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,473 per gram for 24 karat gold, ₹12,350 per gram for 22 karat gold and ₹10,105 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -863,7 +869,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B89"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1588,6 +1594,14 @@
         <v>140</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="s" s="3">
+        <v>142</v>
+      </c>
+      <c r="B90" t="s" s="4">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-16 06:36:26
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="146">
   <si>
     <t>Date</t>
   </si>
@@ -468,6 +468,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,473 per gram for 24 karat gold, ₹12,350 per gram for 22 karat gold and ₹10,105 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>16-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,386 per gram for 24 karat gold, ₹12,270 per gram for 22 karat gold and ₹10,039 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -869,7 +875,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1602,6 +1608,14 @@
         <v>143</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="s" s="3">
+        <v>144</v>
+      </c>
+      <c r="B91" t="s" s="4">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-17 06:35:50
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -474,6 +474,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,386 per gram for 24 karat gold, ₹12,270 per gram for 22 karat gold and ₹10,039 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>17-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,451 per gram for 24 karat gold, ₹12,330 per gram for 22 karat gold and ₹10,088 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -875,7 +881,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1616,6 +1622,14 @@
         <v>145</v>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="s" s="3">
+        <v>146</v>
+      </c>
+      <c r="B92" t="s" s="4">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-18 06:35:34
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="150">
   <si>
     <t>Date</t>
   </si>
@@ -480,6 +480,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,451 per gram for 24 karat gold, ₹12,330 per gram for 22 karat gold and ₹10,088 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>18-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,484 per gram for 24 karat gold, ₹12,360 per gram for 22 karat gold and ₹10,113 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -881,7 +887,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1630,6 +1636,14 @@
         <v>147</v>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" t="s" s="3">
+        <v>148</v>
+      </c>
+      <c r="B93" t="s" s="4">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-19 06:33:44
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="152">
   <si>
     <t>Date</t>
   </si>
@@ -486,6 +486,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,484 per gram for 24 karat gold, ₹12,360 per gram for 22 karat gold and ₹10,113 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>19-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,418 per gram for 24 karat gold, ₹12,300 per gram for 22 karat gold and ₹10,064 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -887,7 +893,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1644,6 +1650,14 @@
         <v>149</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="s" s="3">
+        <v>150</v>
+      </c>
+      <c r="B94" t="s" s="4">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-20 06:32:34
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="153">
   <si>
     <t>Date</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,418 per gram for 24 karat gold, ₹12,300 per gram for 22 karat gold and ₹10,064 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>20-12-2025</t>
   </si>
 </sst>
 </file>
@@ -893,7 +896,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1658,6 +1661,14 @@
         <v>151</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" t="s" s="3">
+        <v>152</v>
+      </c>
+      <c r="B95" t="s" s="4">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-21 06:32:16
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="154">
   <si>
     <t>Date</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>20-12-2025</t>
+  </si>
+  <si>
+    <t>21-12-2025</t>
   </si>
 </sst>
 </file>
@@ -896,7 +899,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1669,6 +1672,14 @@
         <v>151</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="s" s="3">
+        <v>153</v>
+      </c>
+      <c r="B96" t="s" s="4">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-22 06:37:11
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="156">
   <si>
     <t>Date</t>
   </si>
@@ -498,6 +498,12 @@
   </si>
   <si>
     <t>21-12-2025</t>
+  </si>
+  <si>
+    <t>22-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,528 per gram for 24 karat gold, ₹12,400 per gram for 22 karat gold and ₹10,146 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -899,7 +905,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:B97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1680,6 +1686,14 @@
         <v>151</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" t="s" s="3">
+        <v>154</v>
+      </c>
+      <c r="B97" t="s" s="4">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-23 06:36:05
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="158">
   <si>
     <t>Date</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,528 per gram for 24 karat gold, ₹12,400 per gram for 22 karat gold and ₹10,146 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>23-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,855 per gram for 24 karat gold, ₹12,700 per gram for 22 karat gold and ₹10,391 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -905,7 +911,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1694,6 +1700,14 @@
         <v>155</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="s" s="3">
+        <v>156</v>
+      </c>
+      <c r="B98" t="s" s="4">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-24 06:36:08
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="160">
   <si>
     <t>Date</t>
   </si>
@@ -510,6 +510,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,855 per gram for 24 karat gold, ₹12,700 per gram for 22 karat gold and ₹10,391 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>24-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,893 per gram for 24 karat gold, ₹12,735 per gram for 22 karat gold and ₹10,420 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -911,7 +917,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B98"/>
+  <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1708,6 +1714,14 @@
         <v>157</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" t="s" s="3">
+        <v>158</v>
+      </c>
+      <c r="B99" t="s" s="4">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-25 06:35:26
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="162">
   <si>
     <t>Date</t>
   </si>
@@ -516,6 +516,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,893 per gram for 24 karat gold, ₹12,735 per gram for 22 karat gold and ₹10,420 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>25-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,925 per gram for 24 karat gold, ₹12,765 per gram for 22 karat gold and ₹10,444 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -917,7 +923,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1722,6 +1728,14 @@
         <v>159</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="s" s="3">
+        <v>160</v>
+      </c>
+      <c r="B100" t="s" s="4">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-26 06:34:47
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="164">
   <si>
     <t>Date</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,925 per gram for 24 karat gold, ₹12,765 per gram for 22 karat gold and ₹10,444 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>26-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,002 per gram for 24 karat gold, ₹12,835 per gram for 22 karat gold and ₹10,502 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -923,7 +929,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1736,6 +1742,14 @@
         <v>161</v>
       </c>
     </row>
+    <row r="101">
+      <c r="A101" t="s" s="3">
+        <v>162</v>
+      </c>
+      <c r="B101" t="s" s="4">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-27 06:32:49
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="166">
   <si>
     <t>Date</t>
   </si>
@@ -528,6 +528,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,002 per gram for 24 karat gold, ₹12,835 per gram for 22 karat gold and ₹10,502 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>27-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,122 per gram for 24 karat gold, ₹12,945 per gram for 22 karat gold and ₹10,592 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -929,7 +935,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1750,6 +1756,14 @@
         <v>163</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="s" s="3">
+        <v>164</v>
+      </c>
+      <c r="B102" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-28 06:33:40
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="167">
   <si>
     <t>Date</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,122 per gram for 24 karat gold, ₹12,945 per gram for 22 karat gold and ₹10,592 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>28-12-2025</t>
   </si>
 </sst>
 </file>
@@ -935,7 +938,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1764,6 +1767,14 @@
         <v>165</v>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" t="s" s="3">
+        <v>166</v>
+      </c>
+      <c r="B103" t="s" s="4">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-29 06:37:24
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="169">
   <si>
     <t>Date</t>
   </si>
@@ -537,6 +537,12 @@
   </si>
   <si>
     <t>28-12-2025</t>
+  </si>
+  <si>
+    <t>29-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,171 per gram for 24 karat gold, ₹12,990 per gram for 22 karat gold and ₹10,628 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -938,7 +944,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B103"/>
+  <dimension ref="A1:B104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1775,6 +1781,14 @@
         <v>165</v>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="s" s="3">
+        <v>167</v>
+      </c>
+      <c r="B104" t="s" s="4">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-30 06:35:28
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="171">
   <si>
     <t>Date</t>
   </si>
@@ -543,6 +543,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,171 per gram for 24 karat gold, ₹12,990 per gram for 22 karat gold and ₹10,628 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>30-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,620 per gram for 24 karat gold, ₹12,485 per gram for 22 karat gold and ₹10,193 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -944,7 +950,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B104"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1789,6 +1795,14 @@
         <v>168</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" t="s" s="3">
+        <v>169</v>
+      </c>
+      <c r="B105" t="s" s="4">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2025-12-31 06:35:43
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="173">
   <si>
     <t>Date</t>
   </si>
@@ -549,6 +549,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,620 per gram for 24 karat gold, ₹12,485 per gram for 22 karat gold and ₹10,193 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>31-12-2025</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,588 per gram for 24 karat gold, ₹12,455 per gram for 22 karat gold and ₹10,191 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -950,7 +956,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1803,6 +1809,14 @@
         <v>170</v>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" t="s" s="3">
+        <v>171</v>
+      </c>
+      <c r="B106" t="s" s="4">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-01 06:35:38
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="175">
   <si>
     <t>Date</t>
   </si>
@@ -555,6 +555,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,588 per gram for 24 karat gold, ₹12,455 per gram for 22 karat gold and ₹10,191 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>01-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,506 per gram for 24 karat gold, ₹12,380 per gram for 22 karat gold and ₹10,129 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -956,7 +962,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B106"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1817,6 +1823,14 @@
         <v>172</v>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="s" s="3">
+        <v>173</v>
+      </c>
+      <c r="B107" t="s" s="4">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-02 06:36:05
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="177">
   <si>
     <t>Date</t>
   </si>
@@ -561,6 +561,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,506 per gram for 24 karat gold, ₹12,380 per gram for 22 karat gold and ₹10,129 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>02-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,620 per gram for 24 karat gold, ₹12,485 per gram for 22 karat gold and ₹10,215 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -962,7 +968,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B107"/>
+  <dimension ref="A1:B108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1831,6 +1837,14 @@
         <v>174</v>
       </c>
     </row>
+    <row r="108">
+      <c r="A108" t="s" s="3">
+        <v>175</v>
+      </c>
+      <c r="B108" t="s" s="4">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-03 06:32:58
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="179">
   <si>
     <t>Date</t>
   </si>
@@ -567,6 +567,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,620 per gram for 24 karat gold, ₹12,485 per gram for 22 karat gold and ₹10,215 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>03-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,582 per gram for 24 karat gold, ₹12,450 per gram for 22 karat gold and ₹10,187 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -968,7 +974,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1845,6 +1851,14 @@
         <v>176</v>
       </c>
     </row>
+    <row r="109">
+      <c r="A109" t="s" s="3">
+        <v>177</v>
+      </c>
+      <c r="B109" t="s" s="4">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-04 06:34:13
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="180">
   <si>
     <t>Date</t>
   </si>
@@ -573,6 +573,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,582 per gram for 24 karat gold, ₹12,450 per gram for 22 karat gold and ₹10,187 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>04-01-2026</t>
   </si>
 </sst>
 </file>
@@ -974,7 +977,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B109"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1859,6 +1862,14 @@
         <v>178</v>
       </c>
     </row>
+    <row r="110">
+      <c r="A110" t="s" s="3">
+        <v>179</v>
+      </c>
+      <c r="B110" t="s" s="4">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-05 06:40:43
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="182">
   <si>
     <t>Date</t>
   </si>
@@ -576,6 +576,12 @@
   </si>
   <si>
     <t>04-01-2026</t>
+  </si>
+  <si>
+    <t>05-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,740 per gram for 24 karat gold, ₹12,595 per gram for 22 karat gold and ₹10,305 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -977,7 +983,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1870,6 +1876,14 @@
         <v>178</v>
       </c>
     </row>
+    <row r="111">
+      <c r="A111" t="s" s="3">
+        <v>180</v>
+      </c>
+      <c r="B111" t="s" s="4">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-06 06:36:58
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="184">
   <si>
     <t>Date</t>
   </si>
@@ -582,6 +582,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,740 per gram for 24 karat gold, ₹12,595 per gram for 22 karat gold and ₹10,305 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>06-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,882 per gram for 24 karat gold, ₹12,725 per gram for 22 karat gold and ₹10,412 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -983,7 +989,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:B112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1884,6 +1890,14 @@
         <v>181</v>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="s" s="3">
+        <v>182</v>
+      </c>
+      <c r="B112" t="s" s="4">
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-07 06:37:11
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="186">
   <si>
     <t>Date</t>
   </si>
@@ -588,6 +588,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,882 per gram for 24 karat gold, ₹12,725 per gram for 22 karat gold and ₹10,412 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>07-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,948 per gram for 24 karat gold, ₹12,785 per gram for 22 karat gold and ₹10,461 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -989,7 +995,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1898,6 +1904,14 @@
         <v>183</v>
       </c>
     </row>
+    <row r="113">
+      <c r="A113" t="s" s="3">
+        <v>184</v>
+      </c>
+      <c r="B113" t="s" s="4">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-08 06:36:44
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="188">
   <si>
     <t>Date</t>
   </si>
@@ -594,6 +594,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,948 per gram for 24 karat gold, ₹12,785 per gram for 22 karat gold and ₹10,461 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>08-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,800 per gram for 24 karat gold, ₹12,650 per gram for 22 karat gold and ₹10,350 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1001,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B113"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1912,6 +1918,14 @@
         <v>185</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="s" s="3">
+        <v>186</v>
+      </c>
+      <c r="B114" t="s" s="4">
+        <v>187</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-09 06:36:22
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="190">
   <si>
     <t>Date</t>
   </si>
@@ -600,6 +600,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,800 per gram for 24 karat gold, ₹12,650 per gram for 22 karat gold and ₹10,350 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>09-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹13,871 per gram for 24 karat gold, ₹12,715 per gram for 22 karat gold and ₹10,403 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1007,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1926,6 +1932,14 @@
         <v>187</v>
       </c>
     </row>
+    <row r="115">
+      <c r="A115" t="s" s="3">
+        <v>188</v>
+      </c>
+      <c r="B115" t="s" s="4">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-10 06:32:38
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="192">
   <si>
     <t>Date</t>
   </si>
@@ -606,6 +606,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹13,871 per gram for 24 karat gold, ₹12,715 per gram for 22 karat gold and ₹10,403 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>10-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,046 per gram for 24 karat gold, ₹12,875 per gram for 22 karat gold and ₹10,534 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1013,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B115"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1940,6 +1946,14 @@
         <v>189</v>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" t="s" s="3">
+        <v>190</v>
+      </c>
+      <c r="B116" t="s" s="4">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-11 06:34:26
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="193">
   <si>
     <t>Date</t>
   </si>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,046 per gram for 24 karat gold, ₹12,875 per gram for 22 karat gold and ₹10,534 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>11-01-2026</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1016,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1954,6 +1957,14 @@
         <v>191</v>
       </c>
     </row>
+    <row r="117">
+      <c r="A117" t="s" s="3">
+        <v>192</v>
+      </c>
+      <c r="B117" t="s" s="4">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-12 06:39:12
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="195">
   <si>
     <t>Date</t>
   </si>
@@ -615,6 +615,12 @@
   </si>
   <si>
     <t>11-01-2026</t>
+  </si>
+  <si>
+    <t>12-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,215 per gram for 24 karat gold, ₹13,030 per gram for 22 karat gold and ₹10,661 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1022,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B117"/>
+  <dimension ref="A1:B118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1965,6 +1971,14 @@
         <v>191</v>
       </c>
     </row>
+    <row r="118">
+      <c r="A118" t="s" s="3">
+        <v>193</v>
+      </c>
+      <c r="B118" t="s" s="4">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-13 06:36:31
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="197">
   <si>
     <t>Date</t>
   </si>
@@ -621,6 +621,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,215 per gram for 24 karat gold, ₹13,030 per gram for 22 karat gold and ₹10,661 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>13-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,253 per gram for 24 karat gold, ₹13,065 per gram for 22 karat gold and ₹10,690 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1028,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B118"/>
+  <dimension ref="A1:B119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1979,6 +1985,14 @@
         <v>194</v>
       </c>
     </row>
+    <row r="119">
+      <c r="A119" t="s" s="3">
+        <v>195</v>
+      </c>
+      <c r="B119" t="s" s="4">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-14 06:36:27
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="199">
   <si>
     <t>Date</t>
   </si>
@@ -627,6 +627,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,253 per gram for 24 karat gold, ₹13,065 per gram for 22 karat gold and ₹10,690 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>14-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,362 per gram for 24 karat gold, ₹13,165 per gram for 22 karat gold and ₹10,772 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1034,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B119"/>
+  <dimension ref="A1:B120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -1993,6 +1999,14 @@
         <v>196</v>
       </c>
     </row>
+    <row r="120">
+      <c r="A120" t="s" s="3">
+        <v>197</v>
+      </c>
+      <c r="B120" t="s" s="4">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-15 06:36:26
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="201">
   <si>
     <t>Date</t>
   </si>
@@ -633,6 +633,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,362 per gram for 24 karat gold, ₹13,165 per gram for 22 karat gold and ₹10,772 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>15-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,318 per gram for 24 karat gold, ₹13,125 per gram for 22 karat gold and ₹10,739 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1040,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B120"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2007,6 +2013,14 @@
         <v>198</v>
       </c>
     </row>
+    <row r="121">
+      <c r="A121" t="s" s="3">
+        <v>199</v>
+      </c>
+      <c r="B121" t="s" s="4">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-16 06:36:49
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="203">
   <si>
     <t>Date</t>
   </si>
@@ -639,6 +639,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,318 per gram for 24 karat gold, ₹13,125 per gram for 22 karat gold and ₹10,739 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>16-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,340 per gram for 24 karat gold, ₹13,145 per gram for 22 karat gold and ₹10,755 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1046,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2021,6 +2027,14 @@
         <v>200</v>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" t="s" s="3">
+        <v>201</v>
+      </c>
+      <c r="B122" t="s" s="4">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-17 06:32:41
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="205">
   <si>
     <t>Date</t>
   </si>
@@ -645,6 +645,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,340 per gram for 24 karat gold, ₹13,145 per gram for 22 karat gold and ₹10,755 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>17-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,378 per gram for 24 karat gold, ₹13,180 per gram for 22 karat gold and ₹10,784 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1052,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B122"/>
+  <dimension ref="A1:B123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2035,6 +2041,14 @@
         <v>202</v>
       </c>
     </row>
+    <row r="123">
+      <c r="A123" t="s" s="3">
+        <v>203</v>
+      </c>
+      <c r="B123" t="s" s="4">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-18 06:33:32
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="206">
   <si>
     <t>Date</t>
   </si>
@@ -651,6 +651,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,378 per gram for 24 karat gold, ₹13,180 per gram for 22 karat gold and ₹10,784 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>18-01-2026</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1055,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B123"/>
+  <dimension ref="A1:B124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2049,6 +2052,14 @@
         <v>204</v>
       </c>
     </row>
+    <row r="124">
+      <c r="A124" t="s" s="3">
+        <v>205</v>
+      </c>
+      <c r="B124" t="s" s="4">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-19 06:40:44
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="208">
   <si>
     <t>Date</t>
   </si>
@@ -654,6 +654,12 @@
   </si>
   <si>
     <t>18-01-2026</t>
+  </si>
+  <si>
+    <t>19-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,569 per gram for 24 karat gold, ₹13,355 per gram for 22 karat gold and ₹10,927 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1061,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B124"/>
+  <dimension ref="A1:B125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2060,6 +2066,14 @@
         <v>204</v>
       </c>
     </row>
+    <row r="125">
+      <c r="A125" t="s" s="3">
+        <v>206</v>
+      </c>
+      <c r="B125" t="s" s="4">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-20 06:39:00
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="210">
   <si>
     <t>Date</t>
   </si>
@@ -660,6 +660,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,569 per gram for 24 karat gold, ₹13,355 per gram for 22 karat gold and ₹10,927 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>20-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹14,728 per gram for 24 karat gold, ₹13,500 per gram for 22 karat gold and ₹11,046 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1067,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B125"/>
+  <dimension ref="A1:B126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2074,6 +2080,14 @@
         <v>207</v>
       </c>
     </row>
+    <row r="126">
+      <c r="A126" t="s" s="3">
+        <v>208</v>
+      </c>
+      <c r="B126" t="s" s="4">
+        <v>209</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-21 06:38:20
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="212">
   <si>
     <t>Date</t>
   </si>
@@ -666,6 +666,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹14,728 per gram for 24 karat gold, ₹13,500 per gram for 22 karat gold and ₹11,046 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>21-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹15,726 per gram for 24 karat gold, ₹14,415 per gram for 22 karat gold and ₹11,794 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1073,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B126"/>
+  <dimension ref="A1:B127"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2088,6 +2094,14 @@
         <v>209</v>
       </c>
     </row>
+    <row r="127">
+      <c r="A127" t="s" s="3">
+        <v>210</v>
+      </c>
+      <c r="B127" t="s" s="4">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-22 06:37:43
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="214">
   <si>
     <t>Date</t>
   </si>
@@ -672,6 +672,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹15,726 per gram for 24 karat gold, ₹14,415 per gram for 22 karat gold and ₹11,794 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>22-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹15,431 per gram for 24 karat gold, ₹14,145 per gram for 22 karat gold and ₹11,573 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1079,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B127"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2102,6 +2108,14 @@
         <v>211</v>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" t="s" s="3">
+        <v>212</v>
+      </c>
+      <c r="B128" t="s" s="4">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-01-29 12:01:23
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="216">
   <si>
     <t>Date</t>
   </si>
@@ -678,6 +678,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹15,431 per gram for 24 karat gold, ₹14,145 per gram for 22 karat gold and ₹11,573 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>29-01-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹17,885 per gram for 24 karat gold, ₹16,395 per gram for 22 karat gold and ₹13,414 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1085,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B128"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2116,6 +2122,14 @@
         <v>213</v>
       </c>
     </row>
+    <row r="129">
+      <c r="A129" t="s" s="3">
+        <v>214</v>
+      </c>
+      <c r="B129" t="s" s="4">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-02-20 06:58:27
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="218">
   <si>
     <t>Date</t>
   </si>
@@ -684,6 +684,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹17,885 per gram for 24 karat gold, ₹16,395 per gram for 22 karat gold and ₹13,414 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>20-02-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹15,617 per gram for 24 karat gold, ₹14,315 per gram for 22 karat gold and ₹11,713 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1091,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B129"/>
+  <dimension ref="A1:B130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2130,6 +2136,14 @@
         <v>215</v>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" t="s" s="3">
+        <v>216</v>
+      </c>
+      <c r="B130" t="s" s="4">
+        <v>217</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-02-21 06:43:24
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="220">
   <si>
     <t>Date</t>
   </si>
@@ -690,6 +690,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹15,617 per gram for 24 karat gold, ₹14,315 per gram for 22 karat gold and ₹11,713 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>21-02-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹15,928 per gram for 24 karat gold, ₹14,600 per gram for 22 karat gold and ₹11,946 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1097,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B130"/>
+  <dimension ref="A1:B131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2144,6 +2150,14 @@
         <v>217</v>
       </c>
     </row>
+    <row r="131">
+      <c r="A131" t="s" s="3">
+        <v>218</v>
+      </c>
+      <c r="B131" t="s" s="4">
+        <v>219</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-02-22 06:52:37
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="221">
   <si>
     <t>Date</t>
   </si>
@@ -696,6 +696,9 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹15,928 per gram for 24 karat gold, ₹14,600 per gram for 22 karat gold and ₹11,946 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>22-02-2026</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1100,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B131"/>
+  <dimension ref="A1:B132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2158,6 +2161,14 @@
         <v>219</v>
       </c>
     </row>
+    <row r="132">
+      <c r="A132" t="s" s="3">
+        <v>220</v>
+      </c>
+      <c r="B132" t="s" s="4">
+        <v>219</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-02-23 07:06:06
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="223">
   <si>
     <t>Date</t>
   </si>
@@ -699,6 +699,12 @@
   </si>
   <si>
     <t>22-02-2026</t>
+  </si>
+  <si>
+    <t>23-02-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹16,135 per gram for 24 karat gold, ₹14,790 per gram for 22 karat gold and ₹12,101 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1106,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B132"/>
+  <dimension ref="A1:B133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2169,6 +2175,14 @@
         <v>219</v>
       </c>
     </row>
+    <row r="133">
+      <c r="A133" t="s" s="3">
+        <v>221</v>
+      </c>
+      <c r="B133" t="s" s="4">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-02-24 07:01:56
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="225">
   <si>
     <t>Date</t>
   </si>
@@ -705,6 +705,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹16,135 per gram for 24 karat gold, ₹14,790 per gram for 22 karat gold and ₹12,101 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>24-02-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹16,178 per gram for 24 karat gold, ₹14,830 per gram for 22 karat gold and ₹12,134 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1112,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B133"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2183,6 +2189,14 @@
         <v>222</v>
       </c>
     </row>
+    <row r="134">
+      <c r="A134" t="s" s="3">
+        <v>223</v>
+      </c>
+      <c r="B134" t="s" s="4">
+        <v>224</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-02-25 07:03:47
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="227">
   <si>
     <t>Date</t>
   </si>
@@ -711,6 +711,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹16,178 per gram for 24 karat gold, ₹14,830 per gram for 22 karat gold and ₹12,134 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>25-02-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹16,189 per gram for 24 karat gold, ₹14,840 per gram for 22 karat gold and ₹12,142 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1118,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B134"/>
+  <dimension ref="A1:B135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2197,6 +2203,14 @@
         <v>224</v>
       </c>
     </row>
+    <row r="135">
+      <c r="A135" t="s" s="3">
+        <v>225</v>
+      </c>
+      <c r="B135" t="s" s="4">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-02-26 07:02:42
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="229">
   <si>
     <t>Date</t>
   </si>
@@ -717,6 +717,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹16,189 per gram for 24 karat gold, ₹14,840 per gram for 22 karat gold and ₹12,142 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>26-02-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹16,168 per gram for 24 karat gold, ₹14,820 per gram for 22 karat gold and ₹12,126 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1124,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B135"/>
+  <dimension ref="A1:B136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2211,6 +2217,14 @@
         <v>226</v>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" t="s" s="3">
+        <v>227</v>
+      </c>
+      <c r="B136" t="s" s="4">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-02-27 06:56:20
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="231">
   <si>
     <t>Date</t>
   </si>
@@ -723,6 +723,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹16,168 per gram for 24 karat gold, ₹14,820 per gram for 22 karat gold and ₹12,126 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>27-02-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹16,157 per gram for 24 karat gold, ₹14,810 per gram for 22 karat gold and ₹12,118 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1130,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B136"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2225,6 +2231,14 @@
         <v>228</v>
       </c>
     </row>
+    <row r="137">
+      <c r="A137" t="s" s="3">
+        <v>229</v>
+      </c>
+      <c r="B137" t="s" s="4">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-02-28 06:40:31
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="233">
   <si>
     <t>Date</t>
   </si>
@@ -729,6 +729,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹16,157 per gram for 24 karat gold, ₹14,810 per gram for 22 karat gold and ₹12,118 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>28-02-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹16,473 per gram for 24 karat gold, ₹15,100 per gram for 22 karat gold and ₹12,355 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1136,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:B138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2239,6 +2245,14 @@
         <v>230</v>
       </c>
     </row>
+    <row r="138">
+      <c r="A138" t="s" s="3">
+        <v>231</v>
+      </c>
+      <c r="B138" t="s" s="4">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-03-01 06:49:38
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="235">
   <si>
     <t>Date</t>
   </si>
@@ -735,6 +735,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹16,473 per gram for 24 karat gold, ₹15,100 per gram for 22 karat gold and ₹12,355 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>01-03-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹17,308 per gram for 24 karat gold, ₹15,865 per gram for 22 karat gold and ₹12,981 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1142,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B138"/>
+  <dimension ref="A1:B139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2253,6 +2259,14 @@
         <v>232</v>
       </c>
     </row>
+    <row r="139">
+      <c r="A139" t="s" s="3">
+        <v>233</v>
+      </c>
+      <c r="B139" t="s" s="4">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel file from GitHub Actions on 2026-03-02 06:59:50
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/GoldData.xlsx
+++ b/src/test/resources/Data/GoldData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="237">
   <si>
     <t>Date</t>
   </si>
@@ -741,6 +741,12 @@
   </si>
   <si>
     <t>The price of gold in India today is ₹17,308 per gram for 24 karat gold, ₹15,865 per gram for 22 karat gold and ₹12,981 per gram for 18 karat gold (also called 999 gold).</t>
+  </si>
+  <si>
+    <t>02-03-2026</t>
+  </si>
+  <si>
+    <t>The price of gold in India today is ₹16,980 per gram for 24 karat gold, ₹15,565 per gram for 22 karat gold and ₹12,735 per gram for 18 karat gold (also called 999 gold).</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1148,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1874148-A194-473D-9A92-69152072B55A}">
-  <dimension ref="A1:B139"/>
+  <dimension ref="A1:B140"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
@@ -2267,6 +2273,14 @@
         <v>234</v>
       </c>
     </row>
+    <row r="140">
+      <c r="A140" t="s" s="3">
+        <v>235</v>
+      </c>
+      <c r="B140" t="s" s="4">
+        <v>236</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>